<commit_message>
stat + excel + pdf + bulksms + paiement done
</commit_message>
<xml_diff>
--- a/Détails commande.xlsx
+++ b/Détails commande.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -65,16 +65,16 @@
     <t>9899999</t>
   </si>
   <si>
+    <t>ZE</t>
+  </si>
+  <si>
+    <t>KK</t>
+  </si>
+  <si>
+    <t>Entrer votre numero</t>
+  </si>
+  <si>
     <t>Entrer votre nom</t>
-  </si>
-  <si>
-    <t>Entrer votre numero</t>
-  </si>
-  <si>
-    <t>ZE</t>
-  </si>
-  <si>
-    <t>KK</t>
   </si>
 </sst>
 </file>
@@ -195,7 +195,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -204,27 +204,95 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>29.0</v>
+        <v>33.0</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
-        <v>18</v>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>